<commit_message>
DYAR % Comparison added
</commit_message>
<xml_diff>
--- a/base football data.xlsx.xlsx
+++ b/base football data.xlsx.xlsx
@@ -4,26 +4,28 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="1170" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="2013 WR by YPC" sheetId="2" r:id="rId1"/>
     <sheet name="Anquan Boldin Game Chart" sheetId="3" r:id="rId2"/>
     <sheet name="Crabtree Game Chart" sheetId="5" r:id="rId3"/>
     <sheet name="Bold Crab Game Chart" sheetId="9" r:id="rId4"/>
+    <sheet name="DYAR Comparison" sheetId="10" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2013 WR by YPC'!$A$6:$N$157</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Anquan Boldin Game Chart'!$A$2:$R$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Bold Crab Game Chart'!$A$5:$C$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Crabtree Game Chart'!$A$2:$R$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'DYAR Comparison'!$A$11:$V$11</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="402">
   <si>
     <t>RK</t>
   </si>
@@ -1135,6 +1137,9 @@
     <t>L 31-34</t>
   </si>
   <si>
+    <t>Year</t>
+  </si>
+  <si>
     <t>Date</t>
   </si>
   <si>
@@ -1153,10 +1158,79 @@
     <t>Games # 1 to 71 For Each Player</t>
   </si>
   <si>
+    <t>Player</t>
+  </si>
+  <si>
+    <t>Crabtree</t>
+  </si>
+  <si>
     <t>YPC -- Crabtree</t>
   </si>
   <si>
     <t>YPC -- Boldin</t>
+  </si>
+  <si>
+    <t>Team</t>
+  </si>
+  <si>
+    <t>Pos</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>GS</t>
+  </si>
+  <si>
+    <t>Rec</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>C%</t>
+  </si>
+  <si>
+    <t>Yds</t>
+  </si>
+  <si>
+    <t>Yd/Rec</t>
+  </si>
+  <si>
+    <t>DYAR</t>
+  </si>
+  <si>
+    <t>Rank</t>
+  </si>
+  <si>
+    <t>YAR</t>
+  </si>
+  <si>
+    <t>DVOA</t>
+  </si>
+  <si>
+    <t>VOA</t>
+  </si>
+  <si>
+    <t>WR</t>
+  </si>
+  <si>
+    <t>Boldin</t>
+  </si>
+  <si>
+    <t>Player Career Year</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>DYAR %</t>
+  </si>
+  <si>
+    <t>Catch %</t>
+  </si>
+  <si>
+    <t>Receptions</t>
   </si>
 </sst>
 </file>
@@ -1166,7 +1240,14 @@
   <numFmts count="1">
     <numFmt numFmtId="168" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1190,7 +1271,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1203,8 +1284,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -1212,21 +1317,47 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="2" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="2" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="2" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -2595,7 +2726,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> vs. Crabtree)</a:t>
+              <a:t> vs. Crabtree) -- First 71 Games Compared</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -3184,44 +3315,11 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
+        <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
         <c:crossAx val="349136784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
@@ -5114,16 +5212,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>133356</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>812555</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>1473</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>80596</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>124558</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -12168,11 +12266,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:R146"/>
+  <dimension ref="A2:R147"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I2" activeCellId="1" sqref="C2:C146 I2:I146"/>
+      <selection pane="bottomLeft" activeCell="E147" sqref="E147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -12187,16 +12285,16 @@
   <sheetData>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>372</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>371</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>198</v>
@@ -12211,7 +12309,7 @@
         <v>5</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>200</v>
@@ -20303,6 +20401,18 @@
       </c>
       <c r="R146" s="1">
         <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E147" s="1">
+        <f>H147/F147</f>
+        <v>13.51171875</v>
+      </c>
+      <c r="F147" s="1">
+        <v>768</v>
+      </c>
+      <c r="H147" s="1">
+        <v>10377</v>
       </c>
     </row>
   </sheetData>
@@ -20318,11 +20428,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:R73"/>
+  <dimension ref="A2:R74"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:R73"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AB17" sqref="AB17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -20349,16 +20459,16 @@
   <sheetData>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>372</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>371</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>198</v>
@@ -20373,7 +20483,7 @@
         <v>5</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>200</v>
@@ -24377,6 +24487,18 @@
       </c>
       <c r="R73" s="1">
         <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E74" s="1">
+        <f>H74/F74</f>
+        <v>12.993730407523511</v>
+      </c>
+      <c r="F74" s="1">
+        <v>319</v>
+      </c>
+      <c r="H74" s="1">
+        <v>4145</v>
       </c>
     </row>
   </sheetData>
@@ -24394,34 +24516,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E26" sqref="E26"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A20" sqref="A20:A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="1"/>
+    <col min="2" max="2" width="20.140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="17.7109375" style="1" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="D2" s="1"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -26012,4 +26134,1239 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:V27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="11" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5703125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5703125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="8.28515625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.140625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="10.42578125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.5703125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>401</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>386</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>400</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>388</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>389</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>390</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>378</v>
+      </c>
+      <c r="B3" s="12">
+        <v>262</v>
+      </c>
+      <c r="C3" s="12">
+        <v>427</v>
+      </c>
+      <c r="D3" s="13">
+        <f>B3/C3</f>
+        <v>0.61358313817330212</v>
+      </c>
+      <c r="E3" s="12">
+        <v>3359</v>
+      </c>
+      <c r="F3" s="12">
+        <v>21</v>
+      </c>
+      <c r="G3" s="14">
+        <v>12.820610687022901</v>
+      </c>
+      <c r="H3" s="12">
+        <v>564</v>
+      </c>
+      <c r="I3" s="15">
+        <v>0.16790711521286106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>396</v>
+      </c>
+      <c r="B4" s="12">
+        <v>779</v>
+      </c>
+      <c r="C4" s="12">
+        <v>1280</v>
+      </c>
+      <c r="D4" s="13">
+        <f>B4/C4</f>
+        <v>0.60859375000000004</v>
+      </c>
+      <c r="E4" s="12">
+        <v>10217</v>
+      </c>
+      <c r="F4" s="12">
+        <v>59</v>
+      </c>
+      <c r="G4" s="14">
+        <v>13.11553273427471</v>
+      </c>
+      <c r="H4" s="12">
+        <v>1589</v>
+      </c>
+      <c r="I4" s="15">
+        <v>0.15552510521679563</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="N11" s="8" t="s">
+        <v>390</v>
+      </c>
+      <c r="O11" s="8" t="s">
+        <v>399</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="R11" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="S11" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="T11" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="U11" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="V11" s="1" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>378</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>398</v>
+      </c>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7">
+        <f>SUM(G14:G17)</f>
+        <v>56</v>
+      </c>
+      <c r="H12" s="7">
+        <f>SUM(H14:H17)</f>
+        <v>262</v>
+      </c>
+      <c r="I12" s="7">
+        <f>SUM(I14:I17)</f>
+        <v>427</v>
+      </c>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7">
+        <f>SUM(K14:K17)</f>
+        <v>3359</v>
+      </c>
+      <c r="L12" s="7">
+        <f>SUM(L14:L17)</f>
+        <v>21</v>
+      </c>
+      <c r="M12" s="10">
+        <f>K12/H12</f>
+        <v>12.820610687022901</v>
+      </c>
+      <c r="N12" s="8">
+        <f>SUM(N14:N17)</f>
+        <v>564</v>
+      </c>
+      <c r="O12" s="9">
+        <f>(SUM(N12+K12)/K12)-1</f>
+        <v>0.16790711521286106</v>
+      </c>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="7"/>
+      <c r="R12" s="7"/>
+      <c r="S12" s="7"/>
+      <c r="T12" s="7"/>
+      <c r="U12" s="7"/>
+      <c r="V12" s="7"/>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>396</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>398</v>
+      </c>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7">
+        <f>SUM(G18:G27)</f>
+        <v>137</v>
+      </c>
+      <c r="H13" s="7">
+        <f>SUM(H18:H27)</f>
+        <v>779</v>
+      </c>
+      <c r="I13" s="7">
+        <f>SUM(I18:I27)</f>
+        <v>1280</v>
+      </c>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7">
+        <f>SUM(K18:K27)</f>
+        <v>10217</v>
+      </c>
+      <c r="L13" s="7">
+        <f>SUM(L18:L27)</f>
+        <v>59</v>
+      </c>
+      <c r="M13" s="10">
+        <f>K13/H13</f>
+        <v>13.11553273427471</v>
+      </c>
+      <c r="N13" s="8">
+        <f>SUM(N18:N27)</f>
+        <v>1589</v>
+      </c>
+      <c r="O13" s="9">
+        <f>(SUM(N13+K13)/K13)-1</f>
+        <v>0.15552510521679563</v>
+      </c>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="7"/>
+      <c r="R13" s="7"/>
+      <c r="S13" s="7"/>
+      <c r="T13" s="7"/>
+      <c r="U13" s="7"/>
+      <c r="V13" s="7"/>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1">
+        <v>2009</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="F14" s="1">
+        <v>11</v>
+      </c>
+      <c r="G14" s="1">
+        <v>11</v>
+      </c>
+      <c r="H14" s="1">
+        <v>48</v>
+      </c>
+      <c r="I14" s="1">
+        <v>86</v>
+      </c>
+      <c r="J14" s="1">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="K14" s="1">
+        <v>625</v>
+      </c>
+      <c r="L14" s="1">
+        <v>2</v>
+      </c>
+      <c r="M14" s="1">
+        <v>13</v>
+      </c>
+      <c r="N14" s="8">
+        <v>-45</v>
+      </c>
+      <c r="O14" s="8"/>
+      <c r="P14" s="1">
+        <v>77</v>
+      </c>
+      <c r="Q14" s="1">
+        <v>-10</v>
+      </c>
+      <c r="R14" s="1">
+        <v>71</v>
+      </c>
+      <c r="S14" s="1">
+        <v>-0.19600000000000001</v>
+      </c>
+      <c r="T14" s="1">
+        <v>75</v>
+      </c>
+      <c r="U14" s="1">
+        <v>-0.14199999999999999</v>
+      </c>
+      <c r="V14" s="1">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="B15" s="1">
+        <v>2</v>
+      </c>
+      <c r="C15" s="1">
+        <v>2010</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="F15" s="1">
+        <v>16</v>
+      </c>
+      <c r="G15" s="1">
+        <v>15</v>
+      </c>
+      <c r="H15" s="1">
+        <v>55</v>
+      </c>
+      <c r="I15" s="1">
+        <v>100</v>
+      </c>
+      <c r="J15" s="1">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="K15" s="1">
+        <v>741</v>
+      </c>
+      <c r="L15" s="1">
+        <v>6</v>
+      </c>
+      <c r="M15" s="1">
+        <v>13.5</v>
+      </c>
+      <c r="N15" s="8">
+        <v>121</v>
+      </c>
+      <c r="O15" s="8"/>
+      <c r="P15" s="1">
+        <v>37</v>
+      </c>
+      <c r="Q15" s="1">
+        <v>116</v>
+      </c>
+      <c r="R15" s="1">
+        <v>38</v>
+      </c>
+      <c r="S15" s="1">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="T15" s="1">
+        <v>43</v>
+      </c>
+      <c r="U15" s="1">
+        <v>2.3E-2</v>
+      </c>
+      <c r="V15" s="1">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="B16" s="1">
+        <v>3</v>
+      </c>
+      <c r="C16" s="1">
+        <v>2011</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="F16" s="1">
+        <v>15</v>
+      </c>
+      <c r="G16" s="1">
+        <v>14</v>
+      </c>
+      <c r="H16" s="1">
+        <v>73</v>
+      </c>
+      <c r="I16" s="1">
+        <v>114</v>
+      </c>
+      <c r="J16" s="1">
+        <v>0.64</v>
+      </c>
+      <c r="K16" s="1">
+        <v>880</v>
+      </c>
+      <c r="L16" s="1">
+        <v>4</v>
+      </c>
+      <c r="M16" s="1">
+        <v>12.1</v>
+      </c>
+      <c r="N16" s="8">
+        <v>154</v>
+      </c>
+      <c r="O16" s="8"/>
+      <c r="P16" s="1">
+        <v>28</v>
+      </c>
+      <c r="Q16" s="1">
+        <v>125</v>
+      </c>
+      <c r="R16" s="1">
+        <v>38</v>
+      </c>
+      <c r="S16" s="1">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="T16" s="1">
+        <v>41</v>
+      </c>
+      <c r="U16" s="1">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="V16" s="1">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="B17" s="1">
+        <v>4</v>
+      </c>
+      <c r="C17" s="1">
+        <v>2012</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="F17" s="1">
+        <v>16</v>
+      </c>
+      <c r="G17" s="1">
+        <v>16</v>
+      </c>
+      <c r="H17" s="1">
+        <v>86</v>
+      </c>
+      <c r="I17" s="1">
+        <v>127</v>
+      </c>
+      <c r="J17" s="1">
+        <v>0.68</v>
+      </c>
+      <c r="K17" s="1">
+        <v>1113</v>
+      </c>
+      <c r="L17" s="1">
+        <v>9</v>
+      </c>
+      <c r="M17" s="1">
+        <v>12.9</v>
+      </c>
+      <c r="N17" s="8">
+        <v>334</v>
+      </c>
+      <c r="O17" s="8"/>
+      <c r="P17" s="1">
+        <v>10</v>
+      </c>
+      <c r="Q17" s="1">
+        <v>336</v>
+      </c>
+      <c r="R17" s="1">
+        <v>9</v>
+      </c>
+      <c r="S17" s="1">
+        <v>0.219</v>
+      </c>
+      <c r="T17" s="1">
+        <v>13</v>
+      </c>
+      <c r="U17" s="1">
+        <v>0.21099999999999999</v>
+      </c>
+      <c r="V17" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1</v>
+      </c>
+      <c r="C18" s="1">
+        <v>2003</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="F18" s="1">
+        <v>16</v>
+      </c>
+      <c r="G18" s="1">
+        <v>16</v>
+      </c>
+      <c r="H18" s="1">
+        <v>101</v>
+      </c>
+      <c r="I18" s="1">
+        <v>165</v>
+      </c>
+      <c r="J18" s="1">
+        <v>0.61</v>
+      </c>
+      <c r="K18" s="1">
+        <v>1377</v>
+      </c>
+      <c r="L18" s="1">
+        <v>8</v>
+      </c>
+      <c r="M18" s="1">
+        <v>13.6</v>
+      </c>
+      <c r="N18" s="8">
+        <v>253</v>
+      </c>
+      <c r="O18" s="8"/>
+      <c r="P18" s="1">
+        <v>12</v>
+      </c>
+      <c r="Q18" s="1">
+        <v>247</v>
+      </c>
+      <c r="R18" s="1">
+        <v>10</v>
+      </c>
+      <c r="S18" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="T18" s="1">
+        <v>30</v>
+      </c>
+      <c r="U18" s="1">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="V18" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="B19" s="1">
+        <v>2</v>
+      </c>
+      <c r="C19" s="1">
+        <v>2004</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="F19" s="1">
+        <v>10</v>
+      </c>
+      <c r="G19" s="1">
+        <v>9</v>
+      </c>
+      <c r="H19" s="1">
+        <v>56</v>
+      </c>
+      <c r="I19" s="1">
+        <v>104</v>
+      </c>
+      <c r="J19" s="1">
+        <v>0.54</v>
+      </c>
+      <c r="K19" s="1">
+        <v>623</v>
+      </c>
+      <c r="L19" s="1">
+        <v>1</v>
+      </c>
+      <c r="M19" s="1">
+        <v>11.1</v>
+      </c>
+      <c r="N19" s="8">
+        <v>-94</v>
+      </c>
+      <c r="O19" s="8"/>
+      <c r="P19" s="1">
+        <v>80</v>
+      </c>
+      <c r="Q19" s="1">
+        <v>-57</v>
+      </c>
+      <c r="R19" s="1">
+        <v>75</v>
+      </c>
+      <c r="S19" s="1">
+        <v>-0.24199999999999999</v>
+      </c>
+      <c r="T19" s="1">
+        <v>77</v>
+      </c>
+      <c r="U19" s="1">
+        <v>-0.19600000000000001</v>
+      </c>
+      <c r="V19" s="1">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="B20" s="1">
+        <v>3</v>
+      </c>
+      <c r="C20" s="1">
+        <v>2005</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="F20" s="1">
+        <v>14</v>
+      </c>
+      <c r="G20" s="1">
+        <v>14</v>
+      </c>
+      <c r="H20" s="1">
+        <v>106</v>
+      </c>
+      <c r="I20" s="1">
+        <v>175</v>
+      </c>
+      <c r="J20" s="1">
+        <v>0.61</v>
+      </c>
+      <c r="K20" s="1">
+        <v>1438</v>
+      </c>
+      <c r="L20" s="1">
+        <v>7</v>
+      </c>
+      <c r="M20" s="1">
+        <v>13.6</v>
+      </c>
+      <c r="N20" s="8">
+        <v>221</v>
+      </c>
+      <c r="O20" s="8"/>
+      <c r="P20" s="1">
+        <v>18</v>
+      </c>
+      <c r="Q20" s="1">
+        <v>263</v>
+      </c>
+      <c r="R20" s="1">
+        <v>13</v>
+      </c>
+      <c r="S20" s="1">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="T20" s="1">
+        <v>38</v>
+      </c>
+      <c r="U20" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="V20" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="B21" s="1">
+        <v>4</v>
+      </c>
+      <c r="C21" s="1">
+        <v>2006</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="F21" s="1">
+        <v>16</v>
+      </c>
+      <c r="G21" s="1">
+        <v>16</v>
+      </c>
+      <c r="H21" s="1">
+        <v>85</v>
+      </c>
+      <c r="I21" s="1">
+        <v>154</v>
+      </c>
+      <c r="J21" s="1">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="K21" s="1">
+        <v>1208</v>
+      </c>
+      <c r="L21" s="1">
+        <v>4</v>
+      </c>
+      <c r="M21" s="1">
+        <v>14.2</v>
+      </c>
+      <c r="N21" s="8">
+        <v>133</v>
+      </c>
+      <c r="O21" s="8"/>
+      <c r="P21" s="1">
+        <v>35</v>
+      </c>
+      <c r="Q21" s="1">
+        <v>135</v>
+      </c>
+      <c r="R21" s="1">
+        <v>33</v>
+      </c>
+      <c r="S21" s="1">
+        <v>-1.4E-2</v>
+      </c>
+      <c r="T21" s="1">
+        <v>49</v>
+      </c>
+      <c r="U21" s="1">
+        <v>-1.2999999999999999E-2</v>
+      </c>
+      <c r="V21" s="1">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="B22" s="1">
+        <v>5</v>
+      </c>
+      <c r="C22" s="1">
+        <v>2007</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="F22" s="1">
+        <v>12</v>
+      </c>
+      <c r="G22" s="1">
+        <v>11</v>
+      </c>
+      <c r="H22" s="1">
+        <v>71</v>
+      </c>
+      <c r="I22" s="1">
+        <v>100</v>
+      </c>
+      <c r="J22" s="1">
+        <v>0.71</v>
+      </c>
+      <c r="K22" s="1">
+        <v>854</v>
+      </c>
+      <c r="L22" s="1">
+        <v>9</v>
+      </c>
+      <c r="M22" s="1">
+        <v>12</v>
+      </c>
+      <c r="N22" s="8">
+        <v>222</v>
+      </c>
+      <c r="O22" s="8"/>
+      <c r="P22" s="1">
+        <v>17</v>
+      </c>
+      <c r="Q22" s="1">
+        <v>231</v>
+      </c>
+      <c r="R22" s="1">
+        <v>15</v>
+      </c>
+      <c r="S22" s="1">
+        <v>0.155</v>
+      </c>
+      <c r="T22" s="1">
+        <v>17</v>
+      </c>
+      <c r="U22" s="1">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="V22" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="B23" s="1">
+        <v>6</v>
+      </c>
+      <c r="C23" s="1">
+        <v>2008</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="F23" s="1">
+        <v>12</v>
+      </c>
+      <c r="G23" s="1">
+        <v>11</v>
+      </c>
+      <c r="H23" s="1">
+        <v>89</v>
+      </c>
+      <c r="I23" s="1">
+        <v>127</v>
+      </c>
+      <c r="J23" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="K23" s="1">
+        <v>1038</v>
+      </c>
+      <c r="L23" s="1">
+        <v>11</v>
+      </c>
+      <c r="M23" s="1">
+        <v>11.7</v>
+      </c>
+      <c r="N23" s="8">
+        <v>268</v>
+      </c>
+      <c r="O23" s="8"/>
+      <c r="P23" s="1">
+        <v>10</v>
+      </c>
+      <c r="Q23" s="1">
+        <v>246</v>
+      </c>
+      <c r="R23" s="1">
+        <v>11</v>
+      </c>
+      <c r="S23" s="1">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="T23" s="1">
+        <v>16</v>
+      </c>
+      <c r="U23" s="1">
+        <v>0.114</v>
+      </c>
+      <c r="V23" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="B24" s="1">
+        <v>7</v>
+      </c>
+      <c r="C24" s="1">
+        <v>2009</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="F24" s="1">
+        <v>15</v>
+      </c>
+      <c r="G24" s="1">
+        <v>15</v>
+      </c>
+      <c r="H24" s="1">
+        <v>85</v>
+      </c>
+      <c r="I24" s="1">
+        <v>128</v>
+      </c>
+      <c r="J24" s="1">
+        <v>0.66</v>
+      </c>
+      <c r="K24" s="1">
+        <v>1034</v>
+      </c>
+      <c r="L24" s="1">
+        <v>5</v>
+      </c>
+      <c r="M24" s="1">
+        <v>12.2</v>
+      </c>
+      <c r="N24" s="8">
+        <v>124</v>
+      </c>
+      <c r="O24" s="8"/>
+      <c r="P24" s="1">
+        <v>38</v>
+      </c>
+      <c r="Q24" s="1">
+        <v>173</v>
+      </c>
+      <c r="R24" s="1">
+        <v>27</v>
+      </c>
+      <c r="S24" s="1">
+        <v>-2E-3</v>
+      </c>
+      <c r="T24" s="1">
+        <v>45</v>
+      </c>
+      <c r="U24" s="1">
+        <v>4.7E-2</v>
+      </c>
+      <c r="V24" s="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="B25" s="1">
+        <v>8</v>
+      </c>
+      <c r="C25" s="1">
+        <v>2010</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="F25" s="1">
+        <v>16</v>
+      </c>
+      <c r="G25" s="1">
+        <v>16</v>
+      </c>
+      <c r="H25" s="1">
+        <v>64</v>
+      </c>
+      <c r="I25" s="1">
+        <v>109</v>
+      </c>
+      <c r="J25" s="1">
+        <v>0.59</v>
+      </c>
+      <c r="K25" s="1">
+        <v>837</v>
+      </c>
+      <c r="L25" s="1">
+        <v>7</v>
+      </c>
+      <c r="M25" s="1">
+        <v>13.1</v>
+      </c>
+      <c r="N25" s="8">
+        <v>156</v>
+      </c>
+      <c r="O25" s="8"/>
+      <c r="P25" s="1">
+        <v>29</v>
+      </c>
+      <c r="Q25" s="1">
+        <v>141</v>
+      </c>
+      <c r="R25" s="1">
+        <v>30</v>
+      </c>
+      <c r="S25" s="1">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="T25" s="1">
+        <v>38</v>
+      </c>
+      <c r="U25" s="1">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="V25" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="B26" s="1">
+        <v>9</v>
+      </c>
+      <c r="C26" s="1">
+        <v>2011</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="F26" s="1">
+        <v>14</v>
+      </c>
+      <c r="G26" s="1">
+        <v>14</v>
+      </c>
+      <c r="H26" s="1">
+        <v>57</v>
+      </c>
+      <c r="I26" s="1">
+        <v>106</v>
+      </c>
+      <c r="J26" s="1">
+        <v>0.54</v>
+      </c>
+      <c r="K26" s="1">
+        <v>887</v>
+      </c>
+      <c r="L26" s="1">
+        <v>3</v>
+      </c>
+      <c r="M26" s="1">
+        <v>15.6</v>
+      </c>
+      <c r="N26" s="8">
+        <v>184</v>
+      </c>
+      <c r="O26" s="8"/>
+      <c r="P26" s="1">
+        <v>23</v>
+      </c>
+      <c r="Q26" s="1">
+        <v>169</v>
+      </c>
+      <c r="R26" s="1">
+        <v>27</v>
+      </c>
+      <c r="S26" s="1">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="T26" s="1">
+        <v>34</v>
+      </c>
+      <c r="U26" s="1">
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="V26" s="1">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="B27" s="1">
+        <v>10</v>
+      </c>
+      <c r="C27" s="1">
+        <v>2012</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="F27" s="1">
+        <v>15</v>
+      </c>
+      <c r="G27" s="1">
+        <v>15</v>
+      </c>
+      <c r="H27" s="1">
+        <v>65</v>
+      </c>
+      <c r="I27" s="1">
+        <v>112</v>
+      </c>
+      <c r="J27" s="1">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="K27" s="1">
+        <v>921</v>
+      </c>
+      <c r="L27" s="1">
+        <v>4</v>
+      </c>
+      <c r="M27" s="1">
+        <v>14.2</v>
+      </c>
+      <c r="N27" s="8">
+        <v>122</v>
+      </c>
+      <c r="O27" s="8"/>
+      <c r="P27" s="1">
+        <v>39</v>
+      </c>
+      <c r="Q27" s="1">
+        <v>133</v>
+      </c>
+      <c r="R27" s="1">
+        <v>32</v>
+      </c>
+      <c r="S27" s="1">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="T27" s="1">
+        <v>35</v>
+      </c>
+      <c r="U27" s="1">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="V27" s="1">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A11:V11">
+    <sortState ref="A4:U17">
+      <sortCondition descending="1" ref="A3"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="G12:L13 N12:N13" formulaRange="1"/>
+    <ignoredError sqref="M12:M13" formula="1" formulaRange="1"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added fivethirtyeight csv, shall use for WR
</commit_message>
<xml_diff>
--- a/base football data.xlsx.xlsx
+++ b/base football data.xlsx.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="1170" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="2013 WR by YPC" sheetId="2" r:id="rId1"/>
@@ -5533,9 +5533,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A2:N157"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B158" sqref="B158"/>
+      <selection pane="bottomLeft" activeCell="H59" sqref="H59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -24517,8 +24517,8 @@
   <dimension ref="A2:D148"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A20" sqref="A20:A21"/>
+      <pane ySplit="4" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G42" sqref="A39:G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -26140,22 +26140,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:V27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <pane ySplit="11" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomLeft" activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="7.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5703125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="9.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="23.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14" style="1" customWidth="1"/>
     <col min="10" max="10" width="9.7109375" style="1" customWidth="1"/>
     <col min="11" max="11" width="8.28515625" style="1" customWidth="1"/>
     <col min="12" max="12" width="5.85546875" style="1" bestFit="1" customWidth="1"/>

</xml_diff>